<commit_message>
feat: Finalización de la gestión de usuarios y su asociación bancaria
Detalles: Se completó la funcionalidad de gestión (CRUD) para Docentes, Proveedores y Estudiantes. Se implementó la lógica necesaria para asociar cuentas bancarias a estos nuevos usuarios.
</commit_message>
<xml_diff>
--- a/Asociaciones.xlsx
+++ b/Asociaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Issei\Desktop\Proyecto Final V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF67596E-F4F8-4F5B-82DC-A63ADD0B4E8B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A251CC-0C37-45ED-8DA3-B5212B484A44}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{455D771F-41F6-4C34-964D-35EA5127736B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="71">
   <si>
     <t>estado</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>tipo_entidad_pagable</t>
+  </si>
+  <si>
+    <t>estado_proveedor</t>
   </si>
 </sst>
 </file>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD6159-2E5A-41A6-B14A-944EC0C12B72}">
   <dimension ref="A14:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,8 +1454,24 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">

</xml_diff>

<commit_message>
feat: Finalización de la gestión de periodos y cursos
Detalles: Se completó la implementación de las funcionalidades CRUD (Crear, Leer, Actualizar, Eliminar) para Periodos Académicos y Cursos.
</commit_message>
<xml_diff>
--- a/Asociaciones.xlsx
+++ b/Asociaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Issei\Desktop\Proyecto Final V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A251CC-0C37-45ED-8DA3-B5212B484A44}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9CAB9E-7880-4C78-9B5B-1AA631C3448A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{455D771F-41F6-4C34-964D-35EA5127736B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="74">
   <si>
     <t>estado</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>estado_proveedor</t>
+  </si>
+  <si>
+    <t>1 a N (recursiva)</t>
+  </si>
+  <si>
+    <t>periodo</t>
+  </si>
+  <si>
+    <t>estado_curso</t>
   </si>
 </sst>
 </file>
@@ -323,8 +332,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE9D44BB-737B-4530-9040-43043639483A}" name="Tabla1" displayName="Tabla1" ref="C14:C110" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="C14:C110" xr:uid="{88DE967E-1675-434C-95AB-9AFDD62BBD9E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE9D44BB-737B-4530-9040-43043639483A}" name="Tabla1" displayName="Tabla1" ref="C14:C113" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="C14:C113" xr:uid="{88DE967E-1675-434C-95AB-9AFDD62BBD9E}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6DE1058F-658A-4B85-9507-467247330BC7}" name="Tabla"/>
   </tableColumns>
@@ -333,8 +342,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E137C85B-4E09-4664-A0BD-36D3160C0A76}" name="Tabla2" displayName="Tabla2" ref="E14:E110" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="E14:E110" xr:uid="{B011BD4E-4FAE-4E12-A839-438FE4E0F15E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E137C85B-4E09-4664-A0BD-36D3160C0A76}" name="Tabla2" displayName="Tabla2" ref="E14:E113" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="E14:E113" xr:uid="{B011BD4E-4FAE-4E12-A839-438FE4E0F15E}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2AF8FD7D-6C8D-4501-94E2-20C4581FE0C2}" name="Tabla"/>
   </tableColumns>
@@ -652,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD6159-2E5A-41A6-B14A-944EC0C12B72}">
-  <dimension ref="A14:K110"/>
+  <dimension ref="A14:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,8 +891,24 @@
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -906,8 +931,24 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -970,99 +1011,115 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="D32" s="4"/>
+      <c r="A32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="A34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
         <v>36</v>
       </c>
-      <c r="F34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E38" t="s">
         <v>31</v>
       </c>
-      <c r="F35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E39" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,64 +1127,32 @@
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" t="s">
-        <v>15</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s">
-        <v>38</v>
-      </c>
       <c r="F42" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" t="s">
-        <v>15</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -1137,13 +1162,13 @@
         <v>18</v>
       </c>
       <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
         <v>26</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" t="s">
-        <v>57</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -1154,13 +1179,13 @@
         <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
         <v>38</v>
@@ -1174,16 +1199,16 @@
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -1197,13 +1222,13 @@
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
@@ -1214,19 +1239,19 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F48" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1234,16 +1259,16 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F49" t="s">
         <v>15</v>
@@ -1257,13 +1282,13 @@
         <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -1274,19 +1299,19 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F51" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1294,19 +1319,19 @@
         <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F52" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1314,16 +1339,16 @@
         <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
         <v>40</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" t="s">
-        <v>53</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -1337,13 +1362,13 @@
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -1354,19 +1379,19 @@
         <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1374,19 +1399,19 @@
         <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1394,19 +1419,19 @@
         <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F57" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1414,43 +1439,59 @@
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C58" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s">
         <v>54</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="F58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E58" t="s">
-        <v>50</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="E59" t="s">
+        <v>55</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F60" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1461,128 +1502,112 @@
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" t="s">
         <v>70</v>
       </c>
-      <c r="F61" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" t="s">
-        <v>29</v>
-      </c>
-      <c r="F62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="5"/>
-      <c r="D63" s="1"/>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="5"/>
-      <c r="D64" s="1"/>
-      <c r="F64" s="5"/>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" t="s">
         <v>18</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>60</v>
-      </c>
-      <c r="F65" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C66" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" t="s">
-        <v>60</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="5"/>
+      <c r="D66" s="1"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" t="s">
-        <v>60</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E67" t="s">
-        <v>50</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="5"/>
+      <c r="D67" s="1"/>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C68" t="s">
+        <v>59</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" t="s">
-        <v>51</v>
-      </c>
       <c r="F68" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,19 +1615,19 @@
         <v>22</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" t="s">
-        <v>48</v>
-      </c>
       <c r="F69" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1613,13 +1638,13 @@
         <v>15</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E70" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>18</v>
@@ -1633,13 +1658,13 @@
         <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E71" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>18</v>
@@ -1650,19 +1675,19 @@
         <v>22</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
         <v>60</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E72" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1673,95 +1698,95 @@
         <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E73" t="s">
+        <v>60</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
+        <v>60</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>62</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" t="s">
         <v>50</v>
       </c>
-      <c r="F73" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="5"/>
-      <c r="D74" s="1"/>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="5"/>
-      <c r="D75" s="1"/>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="5"/>
-      <c r="D76" s="1"/>
-      <c r="F76" s="5"/>
+      <c r="F76" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C77" t="s">
-        <v>43</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" t="s">
-        <v>44</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="5"/>
+      <c r="D77" s="1"/>
+      <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78" t="s">
-        <v>44</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E78" t="s">
-        <v>45</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="5"/>
+      <c r="D78" s="1"/>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" t="s">
-        <v>46</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" t="s">
-        <v>47</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="5"/>
+      <c r="D79" s="1"/>
+      <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -1771,13 +1796,13 @@
         <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>15</v>
@@ -1788,19 +1813,19 @@
         <v>22</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E81" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,19 +1833,19 @@
         <v>22</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -1828,44 +1853,98 @@
         <v>22</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C83" t="s">
+        <v>48</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>47</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
         <v>49</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="F84" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" t="s">
+        <v>49</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E85" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E86" t="s">
         <v>44</v>
       </c>
-      <c r="F83" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="5"/>
-      <c r="D84" s="1"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="5"/>
-      <c r="D85" s="1"/>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="5"/>
-      <c r="D86" s="1"/>
-      <c r="F86" s="5"/>
+      <c r="F86" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
-      <c r="B87" s="5"/>
-      <c r="D87" s="1"/>
-      <c r="F87" s="5"/>
+      <c r="B87" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E87" t="s">
+        <v>44</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
@@ -1877,66 +1956,69 @@
       <c r="A89" s="1"/>
       <c r="B89" s="5"/>
       <c r="D89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" t="s">
-        <v>50</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90" t="s">
-        <v>51</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="5"/>
+      <c r="D90" s="1"/>
+      <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C91" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E91" t="s">
-        <v>51</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="5"/>
+      <c r="D91" s="1"/>
+      <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="5"/>
       <c r="D92" s="1"/>
-      <c r="F92" s="5"/>
+      <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="F93" s="5"/>
+      <c r="A93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" t="s">
+        <v>51</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="F94" s="5"/>
+      <c r="A94" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" t="s">
+        <v>50</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" t="s">
+        <v>51</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
+      <c r="B95" s="5"/>
       <c r="D95" s="1"/>
       <c r="F95" s="5"/>
     </row>
@@ -1953,124 +2035,111 @@
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="D98" s="1"/>
-      <c r="F98" s="1"/>
+      <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B99" t="s">
-        <v>18</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="A99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102" t="s">
         <v>66</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="D102" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" t="s">
         <v>65</v>
       </c>
-      <c r="F99" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B100" t="s">
-        <v>18</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="F102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B103" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" t="s">
         <v>27</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="D103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" t="s">
         <v>65</v>
       </c>
-      <c r="F100" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B101" t="s">
-        <v>18</v>
-      </c>
-      <c r="C101" t="s">
-        <v>67</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" t="s">
-        <v>65</v>
-      </c>
-      <c r="F101" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="F103" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B104" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E104" t="s">
         <v>65</v>
       </c>
       <c r="F104" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B105" t="s">
-        <v>18</v>
-      </c>
-      <c r="C105" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" t="s">
-        <v>65</v>
-      </c>
-      <c r="F105" t="s">
-        <v>15</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="A107" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B107" t="s">
+        <v>63</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" t="s">
+        <v>65</v>
+      </c>
+      <c r="F107" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
@@ -2080,13 +2149,13 @@
         <v>18</v>
       </c>
       <c r="C108" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E108" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F108" t="s">
         <v>15</v>
@@ -2097,7 +2166,35 @@
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
       <c r="D110" s="1"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B111" t="s">
+        <v>18</v>
+      </c>
+      <c r="C111" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" t="s">
+        <v>68</v>
+      </c>
+      <c r="F111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="D112" s="1"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Implementación completa de reportes gráficos dinámicos
Detalles: Se finalizaron los reportes gráficos dinámicos con opciones de filtrado para las secciones clave del sistema: Entidades, Docentes, Estudiantes, Proveedores y Cuentas Bancarias.
</commit_message>
<xml_diff>
--- a/Asociaciones.xlsx
+++ b/Asociaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Issei\Desktop\Proyecto Final V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9CAB9E-7880-4C78-9B5B-1AA631C3448A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6561200-D531-46A4-ACFC-BCC468C914E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{455D771F-41F6-4C34-964D-35EA5127736B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="74">
   <si>
     <t>estado</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>inscripcion</t>
-  </si>
-  <si>
-    <t>tarifa_docente_grupo</t>
   </si>
   <si>
     <t>unique la columna  en el archivo del belongsTo.  El hasOne debe estar en el lado donde se tenga
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t>estado_curso</t>
+  </si>
+  <si>
+    <t>modalidad_clase</t>
   </si>
 </sst>
 </file>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD6159-2E5A-41A6-B14A-944EC0C12B72}">
   <dimension ref="A14:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +717,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -729,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>8</v>
@@ -741,7 +741,7 @@
         <v>17</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -785,13 +785,13 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="J17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
         <v>18</v>
@@ -941,7 +941,7 @@
         <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
@@ -1038,7 +1038,7 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
@@ -1110,7 +1110,7 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>24</v>
@@ -1123,8 +1123,24 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
@@ -1175,24 +1191,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" t="s">
-        <v>15</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1208,7 +1208,7 @@
         <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -1228,7 +1228,7 @@
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
@@ -1255,24 +1255,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" t="s">
-        <v>15</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -1282,13 +1266,13 @@
         <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -1302,13 +1286,13 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" t="s">
         <v>18</v>
@@ -1322,13 +1306,13 @@
         <v>18</v>
       </c>
       <c r="C52" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
         <v>56</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" t="s">
-        <v>57</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
@@ -1408,7 +1392,7 @@
         <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -1422,13 +1406,13 @@
         <v>18</v>
       </c>
       <c r="C57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
         <v>52</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" t="s">
-        <v>53</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -1442,13 +1426,13 @@
         <v>18</v>
       </c>
       <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s">
         <v>53</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" t="s">
-        <v>54</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -1462,13 +1446,13 @@
         <v>15</v>
       </c>
       <c r="C59" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" t="s">
         <v>54</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E59" t="s">
-        <v>55</v>
       </c>
       <c r="F59" t="s">
         <v>18</v>
@@ -1482,13 +1466,13 @@
         <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F60" t="s">
         <v>18</v>
@@ -1502,13 +1486,13 @@
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F61" t="s">
         <v>18</v>
@@ -1552,7 +1536,7 @@
         <v>24</v>
       </c>
       <c r="E64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F64" t="s">
         <v>18</v>
@@ -1598,13 +1582,13 @@
         <v>18</v>
       </c>
       <c r="C68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
         <v>59</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" t="s">
-        <v>60</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>15</v>
@@ -1624,7 +1608,7 @@
         <v>9</v>
       </c>
       <c r="E69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>15</v>
@@ -1638,13 +1622,13 @@
         <v>15</v>
       </c>
       <c r="C70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>18</v>
@@ -1658,13 +1642,13 @@
         <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>18</v>
@@ -1678,13 +1662,13 @@
         <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>18</v>
@@ -1698,13 +1682,13 @@
         <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>18</v>
@@ -1718,13 +1702,13 @@
         <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E74" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>18</v>
@@ -1738,13 +1722,13 @@
         <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>15</v>
@@ -1758,13 +1742,13 @@
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E76" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>18</v>
@@ -1796,13 +1780,13 @@
         <v>18</v>
       </c>
       <c r="C80" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s">
         <v>43</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" t="s">
-        <v>44</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>15</v>
@@ -1816,13 +1800,13 @@
         <v>15</v>
       </c>
       <c r="C81" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" t="s">
         <v>44</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E81" t="s">
-        <v>45</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>18</v>
@@ -1836,13 +1820,13 @@
         <v>18</v>
       </c>
       <c r="C82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
         <v>46</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" t="s">
-        <v>47</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>15</v>
@@ -1856,13 +1840,13 @@
         <v>18</v>
       </c>
       <c r="C83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>15</v>
@@ -1876,13 +1860,13 @@
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>15</v>
@@ -1896,13 +1880,13 @@
         <v>15</v>
       </c>
       <c r="C85" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E85" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>18</v>
@@ -1916,13 +1900,13 @@
         <v>15</v>
       </c>
       <c r="C86" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E86" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>18</v>
@@ -1934,13 +1918,13 @@
         <v>18</v>
       </c>
       <c r="C87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>15</v>
@@ -1984,13 +1968,13 @@
         <v>15</v>
       </c>
       <c r="C93" t="s">
+        <v>49</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" t="s">
         <v>50</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93" t="s">
-        <v>51</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>18</v>
@@ -2004,13 +1988,13 @@
         <v>15</v>
       </c>
       <c r="C94" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" t="s">
         <v>50</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E94" t="s">
-        <v>51</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>18</v>
@@ -2060,13 +2044,13 @@
         <v>18</v>
       </c>
       <c r="C102" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E102" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F102" t="s">
         <v>15</v>
@@ -2086,7 +2070,7 @@
         <v>9</v>
       </c>
       <c r="E103" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F103" t="s">
         <v>15</v>
@@ -2100,13 +2084,13 @@
         <v>18</v>
       </c>
       <c r="C104" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F104" t="s">
         <v>15</v>
@@ -2126,7 +2110,7 @@
         <v>22</v>
       </c>
       <c r="B107" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2135,10 +2119,10 @@
         <v>10</v>
       </c>
       <c r="E107" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F107" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2155,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="E108" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F108" t="s">
         <v>15</v>
@@ -2177,13 +2161,13 @@
         <v>18</v>
       </c>
       <c r="C111" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E111" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F111" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
feat: Finalización de grupos, inscripciones y mejoras de accesibilidad
Detalles: Se completó la gestión de Grupos, incluyendo la asociación de Docentes a grupos y la inscripción de Estudiantes a grupos (accesibles desde las páginas de detalle correspondientes). Además, se implementaron mejoras para permitir el acceso al sistema desde otros dispositivos y se actualizaron el logo y el nombre del sistema.
</commit_message>
<xml_diff>
--- a/Asociaciones.xlsx
+++ b/Asociaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Issei\Desktop\Proyecto Final V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6561200-D531-46A4-ACFC-BCC468C914E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51475E3-D3EC-4B2E-B12E-E98F5EB8DDFD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{455D771F-41F6-4C34-964D-35EA5127736B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="68">
   <si>
     <t>estado</t>
   </si>
@@ -126,19 +126,10 @@
     <t>categoria_curso</t>
   </si>
   <si>
-    <t>bloque_horario</t>
-  </si>
-  <si>
-    <t>dia</t>
-  </si>
-  <si>
     <t>estado_grupo</t>
   </si>
   <si>
     <t>grupo</t>
-  </si>
-  <si>
-    <t>asignacion_horario_grupo</t>
   </si>
   <si>
     <t>asignacion_docente</t>
@@ -163,9 +154,6 @@
     <t>naturaleza</t>
   </si>
   <si>
-    <t>fuente_asiento</t>
-  </si>
-  <si>
     <t>asiento_encabezado</t>
   </si>
   <si>
@@ -181,39 +169,12 @@
     <t>divisa</t>
   </si>
   <si>
-    <t>estado_plan</t>
-  </si>
-  <si>
-    <t>plan_pago</t>
-  </si>
-  <si>
-    <t>pagos_estudiantes</t>
-  </si>
-  <si>
-    <t>tipo_pago</t>
-  </si>
-  <si>
     <t>liquidacion_nomina</t>
   </si>
   <si>
     <t>registro_horas</t>
   </si>
   <si>
-    <t>pagos_docentes</t>
-  </si>
-  <si>
-    <t>estado_factura</t>
-  </si>
-  <si>
-    <t>facturas_gasto</t>
-  </si>
-  <si>
-    <t>detalle_factura</t>
-  </si>
-  <si>
-    <t>pagos_proveedores</t>
-  </si>
-  <si>
     <t>belongsToMany</t>
   </si>
   <si>
@@ -248,6 +209,27 @@
   </si>
   <si>
     <t>modalidad_clase</t>
+  </si>
+  <si>
+    <t>obligacion_financiera</t>
+  </si>
+  <si>
+    <t>estado_obligacion</t>
+  </si>
+  <si>
+    <t>concepto_financiero</t>
+  </si>
+  <si>
+    <t>obligacion_inscripcion</t>
+  </si>
+  <si>
+    <t>registro_transaccion</t>
+  </si>
+  <si>
+    <t>tipo_movimiento</t>
+  </si>
+  <si>
+    <t>metodo_pago</t>
   </si>
 </sst>
 </file>
@@ -332,8 +314,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE9D44BB-737B-4530-9040-43043639483A}" name="Tabla1" displayName="Tabla1" ref="C14:C113" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="C14:C113" xr:uid="{88DE967E-1675-434C-95AB-9AFDD62BBD9E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE9D44BB-737B-4530-9040-43043639483A}" name="Tabla1" displayName="Tabla1" ref="C14:C143" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="C14:C143" xr:uid="{88DE967E-1675-434C-95AB-9AFDD62BBD9E}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6DE1058F-658A-4B85-9507-467247330BC7}" name="Tabla"/>
   </tableColumns>
@@ -342,8 +324,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E137C85B-4E09-4664-A0BD-36D3160C0A76}" name="Tabla2" displayName="Tabla2" ref="E14:E113" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="E14:E113" xr:uid="{B011BD4E-4FAE-4E12-A839-438FE4E0F15E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E137C85B-4E09-4664-A0BD-36D3160C0A76}" name="Tabla2" displayName="Tabla2" ref="E14:E143" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="E14:E143" xr:uid="{B011BD4E-4FAE-4E12-A839-438FE4E0F15E}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2AF8FD7D-6C8D-4501-94E2-20C4581FE0C2}" name="Tabla"/>
   </tableColumns>
@@ -661,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD6159-2E5A-41A6-B14A-944EC0C12B72}">
-  <dimension ref="A14:K113"/>
+  <dimension ref="A14:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +699,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -729,7 +711,7 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>8</v>
@@ -741,7 +723,7 @@
         <v>17</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -785,13 +767,13 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -904,7 +886,7 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
         <v>18</v>
@@ -941,7 +923,7 @@
         <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
@@ -951,64 +933,16 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" t="s">
-        <v>18</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" t="s">
-        <v>15</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1024,7 +958,7 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -1038,13 +972,13 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -1070,13 +1004,13 @@
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -1090,7 +1024,7 @@
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>24</v>
@@ -1110,13 +1044,13 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F39" t="s">
         <v>18</v>
@@ -1130,13 +1064,13 @@
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="F40" t="s">
         <v>18</v>
@@ -1208,7 +1142,7 @@
         <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -1228,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
@@ -1242,13 +1176,13 @@
         <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F48" t="s">
         <v>15</v>
@@ -1259,64 +1193,16 @@
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" t="s">
-        <v>15</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" t="s">
-        <v>49</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" t="s">
-        <v>56</v>
-      </c>
-      <c r="F52" t="s">
-        <v>15</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -1326,13 +1212,13 @@
         <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -1352,7 +1238,7 @@
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -1366,137 +1252,41 @@
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F55" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" t="s">
-        <v>52</v>
-      </c>
-      <c r="F56" t="s">
-        <v>15</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" t="s">
-        <v>52</v>
-      </c>
-      <c r="F57" t="s">
-        <v>15</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>18</v>
-      </c>
-      <c r="C58" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" t="s">
-        <v>53</v>
-      </c>
-      <c r="F58" t="s">
-        <v>15</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E59" t="s">
-        <v>54</v>
-      </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B60" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" t="s">
-        <v>50</v>
-      </c>
-      <c r="F60" t="s">
-        <v>18</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" t="s">
-        <v>49</v>
-      </c>
-      <c r="F61" t="s">
-        <v>18</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
@@ -1536,7 +1326,7 @@
         <v>24</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F64" t="s">
         <v>18</v>
@@ -1575,184 +1365,58 @@
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C68" t="s">
-        <v>58</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" t="s">
-        <v>59</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="5"/>
+      <c r="D68" s="1"/>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" t="s">
-        <v>59</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="5"/>
+      <c r="D69" s="1"/>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" t="s">
-        <v>49</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="5"/>
+      <c r="D70" s="1"/>
+      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" t="s">
-        <v>59</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" t="s">
-        <v>50</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="5"/>
+      <c r="D71" s="1"/>
+      <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" t="s">
-        <v>59</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E72" t="s">
-        <v>47</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="5"/>
+      <c r="D72" s="1"/>
+      <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" t="s">
-        <v>60</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E73" t="s">
-        <v>59</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="5"/>
+      <c r="D73" s="1"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" t="s">
-        <v>60</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E74" t="s">
-        <v>43</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="5"/>
+      <c r="D74" s="1"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C75" t="s">
-        <v>59</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" t="s">
-        <v>61</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="D75" s="1"/>
+      <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" t="s">
-        <v>61</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E76" t="s">
-        <v>49</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="5"/>
+      <c r="D76" s="1"/>
+      <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
@@ -1780,13 +1444,13 @@
         <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>15</v>
@@ -1800,37 +1464,23 @@
         <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E81" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C82" t="s">
-        <v>45</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" t="s">
-        <v>46</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="5"/>
+      <c r="D82" s="1"/>
+      <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
@@ -1840,13 +1490,13 @@
         <v>18</v>
       </c>
       <c r="C83" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>15</v>
@@ -1860,13 +1510,13 @@
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>15</v>
@@ -1880,13 +1530,13 @@
         <v>15</v>
       </c>
       <c r="C85" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E85" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>18</v>
@@ -1900,13 +1550,13 @@
         <v>15</v>
       </c>
       <c r="C86" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E86" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>18</v>
@@ -1918,13 +1568,13 @@
         <v>18</v>
       </c>
       <c r="C87" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E87" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>15</v>
@@ -1968,13 +1618,13 @@
         <v>15</v>
       </c>
       <c r="C93" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E93" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>18</v>
@@ -1988,13 +1638,13 @@
         <v>15</v>
       </c>
       <c r="C94" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E94" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>18</v>
@@ -2044,13 +1694,13 @@
         <v>18</v>
       </c>
       <c r="C102" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E102" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F102" t="s">
         <v>15</v>
@@ -2070,7 +1720,7 @@
         <v>9</v>
       </c>
       <c r="E103" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F103" t="s">
         <v>15</v>
@@ -2084,13 +1734,13 @@
         <v>18</v>
       </c>
       <c r="C104" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F104" t="s">
         <v>15</v>
@@ -2110,7 +1760,7 @@
         <v>22</v>
       </c>
       <c r="B107" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2119,10 +1769,10 @@
         <v>10</v>
       </c>
       <c r="E107" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F107" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2139,7 +1789,7 @@
         <v>9</v>
       </c>
       <c r="E108" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F108" t="s">
         <v>15</v>
@@ -2161,13 +1811,13 @@
         <v>18</v>
       </c>
       <c r="C111" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E111" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F111" t="s">
         <v>15</v>
@@ -2177,8 +1827,368 @@
       <c r="A112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
       <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="D114" s="1"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="D115" s="1"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="D116" s="1"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="D117" s="1"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="D118" s="1"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B119" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" t="s">
+        <v>61</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E119" t="s">
+        <v>62</v>
+      </c>
+      <c r="F119" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B120" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" t="s">
+        <v>61</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E120" t="s">
+        <v>5</v>
+      </c>
+      <c r="F120" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B121" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" t="s">
+        <v>61</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E121" t="s">
+        <v>63</v>
+      </c>
+      <c r="F121" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B122" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" t="s">
+        <v>61</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E122" t="s">
+        <v>43</v>
+      </c>
+      <c r="F122" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B123" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" t="s">
+        <v>61</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E123" t="s">
+        <v>46</v>
+      </c>
+      <c r="F123" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B124" t="s">
+        <v>14</v>
+      </c>
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" t="s">
+        <v>64</v>
+      </c>
+      <c r="F124" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B125" t="s">
+        <v>18</v>
+      </c>
+      <c r="C125" t="s">
+        <v>63</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E125" t="s">
+        <v>63</v>
+      </c>
+      <c r="F125" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="D126" s="1"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+      <c r="D127" s="1"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+      <c r="D128" s="1"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B129" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" t="s">
+        <v>64</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E129" t="s">
+        <v>37</v>
+      </c>
+      <c r="F129" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="D131" s="1"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="D132" s="1"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="D133" s="1"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="D134" s="1"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B135" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135" t="s">
+        <v>65</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E135" t="s">
+        <v>61</v>
+      </c>
+      <c r="F135" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B136" t="s">
+        <v>15</v>
+      </c>
+      <c r="C136" t="s">
+        <v>65</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E136" t="s">
+        <v>5</v>
+      </c>
+      <c r="F136" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B137" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" t="s">
+        <v>65</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E137" t="s">
+        <v>66</v>
+      </c>
+      <c r="F137" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B138" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" t="s">
+        <v>65</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E138" t="s">
+        <v>67</v>
+      </c>
+      <c r="F138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B139" t="s">
+        <v>15</v>
+      </c>
+      <c r="C139" t="s">
+        <v>65</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E139" t="s">
+        <v>46</v>
+      </c>
+      <c r="F139" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="D140" s="1"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="D141" s="1"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B142" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" t="s">
+        <v>42</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E142" t="s">
+        <v>61</v>
+      </c>
+      <c r="F142" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B143" t="s">
+        <v>15</v>
+      </c>
+      <c r="C143" t="s">
+        <v>42</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E143" t="s">
+        <v>65</v>
+      </c>
+      <c r="F143" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: Cierre del desarrollo para la fecha de entrega
Detalles: Se registra el estado final del sistema para cumplir con la fecha límite de entrega. Aunque se reconoce la existencia de funcionalidades pendientes, esta versión representa el producto final para la evaluación.
</commit_message>
<xml_diff>
--- a/Asociaciones.xlsx
+++ b/Asociaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Issei\Desktop\Proyecto Final V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51475E3-D3EC-4B2E-B12E-E98F5EB8DDFD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFB1674-4956-42E4-BAB2-094B965086E3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{455D771F-41F6-4C34-964D-35EA5127736B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="69">
   <si>
     <t>estado</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>metodo_pago</t>
+  </si>
+  <si>
+    <t>transaccion_bancaria</t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD6159-2E5A-41A6-B14A-944EC0C12B72}">
   <dimension ref="A14:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:F31"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,12 +1831,44 @@
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="D113" s="1"/>
+      <c r="A113" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B113" t="s">
+        <v>18</v>
+      </c>
+      <c r="C113" t="s">
+        <v>51</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" t="s">
+        <v>68</v>
+      </c>
+      <c r="F113" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="D114" s="1"/>
+      <c r="A114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B114" t="s">
+        <v>18</v>
+      </c>
+      <c r="C114" t="s">
+        <v>51</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" t="s">
+        <v>68</v>
+      </c>
+      <c r="F114" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
@@ -1992,8 +2027,24 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-      <c r="D126" s="1"/>
+      <c r="A126" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B126" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" t="s">
+        <v>63</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E126" t="s">
+        <v>40</v>
+      </c>
+      <c r="F126" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
@@ -2143,8 +2194,24 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
-      <c r="D140" s="1"/>
+      <c r="A140" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B140" t="s">
+        <v>14</v>
+      </c>
+      <c r="C140" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" t="s">
+        <v>68</v>
+      </c>
+      <c r="F140" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>

</xml_diff>